<commit_message>
Add data of last update to xlsx
</commit_message>
<xml_diff>
--- a/swe-corona.xlsx
+++ b/swe-corona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\Documents\scratch.local\swe-corona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9816D9BE-283F-45D2-9A1D-0F253B362CDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B4E4BD-3AE4-47C2-BF58-B7CC0B176EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38385" yWindow="4395" windowWidth="38370" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Gesamt</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>/100k (7Tage)</t>
+  </si>
+  <si>
+    <t>Last Update: 06/08/2020 14:00:04</t>
   </si>
 </sst>
 </file>
@@ -1602,6 +1605,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
       <c r="AJ1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Render plot as image
</commit_message>
<xml_diff>
--- a/swe-corona.xlsx
+++ b/swe-corona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\Documents\scratch.local\swe-corona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35729BF1-A1E0-435C-800F-214396593A82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55D4304-861E-4B04-B2A4-C186A57660C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38385" yWindow="4395" windowWidth="38370" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
     <t>/100k (7Tage)</t>
   </si>
   <si>
-    <t>Last Update: 06/08/2020 15:49:41</t>
+    <t>Last Update: 06/08/2020 17:53:35</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1588,7 @@
   <dimension ref="A1:AJ996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add date of last update to png
</commit_message>
<xml_diff>
--- a/swe-corona.xlsx
+++ b/swe-corona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\Documents\scratch.local\swe-corona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55D4304-861E-4B04-B2A4-C186A57660C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F4FDAB-2C98-40D6-BBCF-B2003DA8452D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38385" yWindow="4395" windowWidth="38370" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
     <t>/100k (7Tage)</t>
   </si>
   <si>
-    <t>Last Update: 06/08/2020 17:53:35</t>
+    <t>Last Update: 06/08/2020 18:01:11</t>
   </si>
 </sst>
 </file>
@@ -261,22 +261,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-DE"/>
-              <a:t>Neuinfektionen</a:t>
+              <a:rPr lang="de-DE"/>
+              <a:t>Neuinfektionen/100k (7 Tage) - Last Update: 06/08/2020 18:01:11</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>/100</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-DE"/>
-              <a:t>k </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t>(7 Tage)</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>

</xml_diff>

<commit_message>
Change how date of last update is named
</commit_message>
<xml_diff>
--- a/swe-corona.xlsx
+++ b/swe-corona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\Documents\scratch.local\swe-corona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F4FDAB-2C98-40D6-BBCF-B2003DA8452D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A555E1-587E-4B91-8249-480B62DE10D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38385" yWindow="4395" windowWidth="38370" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,7 @@
     <t>/100k (7Tage)</t>
   </si>
   <si>
-    <t>Last Update: 06/08/2020 18:01:11</t>
+    <t>Datenabruf: 06/08/2020 20:39:50</t>
   </si>
 </sst>
 </file>
@@ -262,7 +262,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Neuinfektionen/100k (7 Tage) - Last Update: 06/08/2020 18:01:11</a:t>
+              <a:t>Neuinfektionen/100k (7 Tage) - Datenabruf: 06/08/2020 20:39:50</a:t>
             </a:r>
           </a:p>
         </c:rich>

</xml_diff>